<commit_message>
add 2018/5/3 log file
</commit_message>
<xml_diff>
--- a/log/log_201508030220_张羽.xlsx
+++ b/log/log_201508030220_张羽.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
   <si>
     <t>日期</t>
   </si>
@@ -67,6 +67,13 @@
   <si>
     <t>1、学习selvet相关内容
 2、把github上Spritnoodle项目替换成log项目</t>
+  </si>
+  <si>
+    <t>19:30-22:30</t>
+  </si>
+  <si>
+    <t>1、学习EL表达式以及JSTL 
+2、学习数据库查询操作</t>
   </si>
   <si>
     <t>周次</t>
@@ -94,6 +101,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
@@ -101,59 +167,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,37 +221,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -216,23 +239,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,6 +254,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -265,24 +332,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -295,43 +344,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,78 +435,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,15 +445,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -480,26 +478,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,6 +498,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,151 +530,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1017,7 +1024,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
@@ -1046,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="54" spans="1:4">
+    <row r="2" ht="40.5" spans="1:4">
       <c r="A2" s="1">
         <v>43216</v>
       </c>
@@ -1098,15 +1105,26 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
-      <c r="C6" s="3"/>
+    <row r="6" ht="27" spans="1:4">
+      <c r="A6" s="1">
+        <v>43223</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1132,13 +1150,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update 2018/5/9 log file
</commit_message>
<xml_diff>
--- a/log/log_201508030220_张羽.xlsx
+++ b/log/log_201508030220_张羽.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
   <si>
     <t>日期</t>
   </si>
@@ -74,6 +74,27 @@
   <si>
     <t>1、学习EL表达式以及JSTL 
 2、学习数据库查询操作</t>
+  </si>
+  <si>
+    <t>9:00-11:00</t>
+  </si>
+  <si>
+    <t>1、学习jsp以及相关内容</t>
+  </si>
+  <si>
+    <t>1、继续学习jsp，servlet以及相关内容</t>
+  </si>
+  <si>
+    <t>1、学习service包</t>
+  </si>
+  <si>
+    <t>1、继续学习service包</t>
+  </si>
+  <si>
+    <t>1、学习spring boot相关内容</t>
+  </si>
+  <si>
+    <t>1、学习使用Srping Test整合JUnit4进行单元测试</t>
   </si>
   <si>
     <t>周次</t>
@@ -101,82 +122,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,6 +152,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,19 +222,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,25 +275,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,78 +432,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,6 +466,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -459,6 +519,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,75 +566,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -563,133 +584,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1021,18 +1042,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="36.625" customWidth="1"/>
-    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="4" max="4" width="32.625" customWidth="1"/>
     <col min="5" max="5" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1122,8 +1143,92 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>43224</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="27" spans="1:4">
+      <c r="A8" s="1">
+        <v>42129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>42130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>42131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>42132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" ht="27" spans="1:4">
+      <c r="A12" s="1">
+        <v>42133</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1150,13 +1255,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update 2018/5/10 log file
</commit_message>
<xml_diff>
--- a/log/log_201508030220_张羽.xlsx
+++ b/log/log_201508030220_张羽.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="18375" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="日志" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28">
   <si>
     <t>日期</t>
   </si>
@@ -95,6 +95,13 @@
   </si>
   <si>
     <t>1、学习使用Srping Test整合JUnit4进行单元测试</t>
+  </si>
+  <si>
+    <t>17:00-19:00</t>
+  </si>
+  <si>
+    <t>1、学习Test类
+2、利用test增加表数据</t>
   </si>
   <si>
     <t>周次</t>
@@ -108,9 +115,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -1042,10 +1049,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1224,11 +1231,25 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="13" ht="27" spans="1:4">
+      <c r="A13" s="1">
+        <v>42134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1255,13 +1276,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update 2018/5/11 log file
</commit_message>
<xml_diff>
--- a/log/log_201508030220_张羽.xlsx
+++ b/log/log_201508030220_张羽.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>日期</t>
   </si>
@@ -102,6 +102,13 @@
   <si>
     <t>1、学习Test类
 2、利用test增加表数据</t>
+  </si>
+  <si>
+    <t>19:00-21:00</t>
+  </si>
+  <si>
+    <t>1、模仿dream中实体类的JUnit Test 
+写出自己实体类的JUnit Test</t>
   </si>
   <si>
     <t>周次</t>
@@ -115,10 +122,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -129,8 +136,98 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,60 +256,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,42 +272,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -282,6 +289,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -312,60 +439,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -373,72 +446,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,26 +483,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,6 +513,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -526,6 +533,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,40 +580,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -591,133 +598,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1049,10 +1056,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1245,11 +1252,25 @@
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="14" ht="27" spans="1:4">
+      <c r="A14" s="1">
+        <v>42135</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1276,13 +1297,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update 2018/5/12 log file
</commit_message>
<xml_diff>
--- a/log/log_201508030220_张羽.xlsx
+++ b/log/log_201508030220_张羽.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18375" windowHeight="10560"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="日志" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>日期</t>
   </si>
@@ -109,6 +109,14 @@
   <si>
     <t>1、模仿dream中实体类的JUnit Test 
 写出自己实体类的JUnit Test</t>
+  </si>
+  <si>
+    <t>21:00-23:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1、学习Hibernate的对象关系映射中
+单向的四种映射
+</t>
   </si>
   <si>
     <t>周次</t>
@@ -122,10 +130,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -136,9 +144,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,16 +158,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -168,6 +167,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -182,37 +196,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,38 +211,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,9 +225,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,6 +297,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -307,6 +333,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -343,19 +387,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,30 +453,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -434,42 +478,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,32 +491,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,8 +503,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,26 +524,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,16 +558,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -598,142 +606,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1056,10 +1061,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1177,7 +1182,7 @@
     </row>
     <row r="8" ht="27" spans="1:4">
       <c r="A8" s="1">
-        <v>42129</v>
+        <v>43225</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1191,7 +1196,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>42130</v>
+        <v>43226</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1205,7 +1210,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>42131</v>
+        <v>43227</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1219,7 +1224,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>42132</v>
+        <v>43228</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1233,7 +1238,7 @@
     </row>
     <row r="12" ht="27" spans="1:4">
       <c r="A12" s="1">
-        <v>42133</v>
+        <v>43229</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1247,7 +1252,7 @@
     </row>
     <row r="13" ht="27" spans="1:4">
       <c r="A13" s="1">
-        <v>42134</v>
+        <v>43230</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -1261,16 +1266,30 @@
     </row>
     <row r="14" ht="27" spans="1:4">
       <c r="A14" s="1">
-        <v>42135</v>
+        <v>43231</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="15" ht="40.5" spans="1:4">
+      <c r="A15" s="1">
+        <v>43232</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1297,13 +1316,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update 2018/5/23 log file
</commit_message>
<xml_diff>
--- a/log/log_201508030220_张羽.xlsx
+++ b/log/log_201508030220_张羽.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
   <si>
     <t>日期</t>
   </si>
@@ -52,7 +52,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">    2018/4/28</t>
+    <t xml:space="preserve">     2018/4/28</t>
   </si>
   <si>
     <t>20:30-22:30</t>
@@ -119,10 +119,83 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">1、学习Hibernate的对象关系映射中
+双向的三种映射
+</t>
+  </si>
+  <si>
+    <t>19:30-21:30</t>
+  </si>
+  <si>
+    <t>1、学习Hibernate的HQL</t>
+  </si>
+  <si>
+    <t>1、继续学习Hibernate的HQL</t>
+  </si>
+  <si>
+    <t>1、接着学习Hibernate的HQL</t>
+  </si>
+  <si>
+    <t>1、用JUnit Test方法在数据库中建表</t>
+  </si>
+  <si>
+    <t>1、整理github上的项目</t>
+  </si>
+  <si>
+    <t>1、学习Hibernate的QBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2018/5/20</t>
+  </si>
+  <si>
+    <t>1、继续学习Hibernate的QBC</t>
+  </si>
+  <si>
+    <t>1、学习Hibernate的原生SQL检索</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2018/5/22</t>
+  </si>
+  <si>
+    <t>1、学习Hibernate的一级缓存</t>
+  </si>
+  <si>
+    <t>1、学习Hibernate的二级缓存</t>
+  </si>
+  <si>
     <t>周次</t>
   </si>
   <si>
     <t>执行情况</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1、学习dream项目中的entity包和dao包
+2、写出自己项目的entity包和dao包
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1、自己项目的dao包尚有欠缺
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1、学习EL表达式以及JSTL 
+2、学习数据库查询操作
+3、学习selvet相关内容
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>1、学习使用Srping Test整合JUnit4进行单元测试
+2、模仿dream中实体类的JUnit Test写出自己实体类的JUnit Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1、用JUnit Test方法在数据库中建表
+2、整理github上的项目
+3、学习Hibernate相关内容
+</t>
   </si>
 </sst>
 </file>
@@ -131,9 +204,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -145,12 +218,110 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -166,75 +337,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,38 +353,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -297,6 +370,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -315,19 +454,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,55 +466,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,79 +532,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,24 +561,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -541,11 +596,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,7 +616,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,10 +667,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -606,16 +679,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -624,124 +697,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1061,18 +1140,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="36.625" customWidth="1"/>
-    <col min="4" max="4" width="32.625" customWidth="1"/>
+    <col min="4" max="4" width="33.375" customWidth="1"/>
     <col min="5" max="5" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1093,203 +1172,376 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="40.5" spans="1:4">
-      <c r="A2" s="1">
+    <row r="2" ht="40.5" spans="1:5">
+      <c r="A2" s="3">
         <v>43216</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" ht="81" spans="1:5">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>43217</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="40.5" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" ht="40.5" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" ht="40.5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="40.5" spans="1:5">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" ht="27" spans="1:4">
-      <c r="A6" s="1">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="27" spans="1:5">
+      <c r="A6" s="3">
         <v>43223</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3">
         <v>43224</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" ht="27" spans="1:4">
-      <c r="A8" s="1">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="27" spans="1:5">
+      <c r="A8" s="3">
         <v>43225</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3">
         <v>43226</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3">
         <v>43227</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3">
         <v>43228</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" ht="27" spans="1:4">
-      <c r="A12" s="1">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" ht="27" spans="1:5">
+      <c r="A12" s="3">
         <v>43229</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" ht="27" spans="1:4">
-      <c r="A13" s="1">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" ht="27" spans="1:5">
+      <c r="A13" s="3">
         <v>43230</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" ht="27" spans="1:4">
-      <c r="A14" s="1">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" ht="27" spans="1:5">
+      <c r="A14" s="3">
         <v>43231</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" ht="40.5" spans="1:4">
-      <c r="A15" s="1">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" ht="40.5" spans="1:5">
+      <c r="A15" s="3">
         <v>43232</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" ht="40.5" spans="1:5">
+      <c r="A16" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3">
+        <v>43234</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3">
+        <v>43235</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3">
+        <v>43236</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3">
+        <v>43237</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3">
+        <v>43238</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4">
+        <v>43239</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4">
+        <v>43241</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4">
+        <v>43243</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1302,41 +1554,147 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
     <col min="4" max="4" width="26.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="77.25" customHeight="1" spans="1:1">
+    <row r="2" ht="78" customHeight="1" spans="1:4">
       <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" ht="89" customHeight="1" spans="1:4">
       <c r="A3">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" ht="96" customHeight="1" spans="1:4">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" ht="93" customHeight="1" spans="1:4">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" ht="48" customHeight="1" spans="1:4">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>